<commit_message>
made a note for the swiss economists abroad conference
thanks for this, it’s great!
</commit_message>
<xml_diff>
--- a/Prospective_Conferences_AY1819.xlsx
+++ b/Prospective_Conferences_AY1819.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\th3\Documents\BG_2017\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24735" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Conference </t>
   </si>
@@ -69,11 +67,14 @@
   <si>
     <t>Midwest macro Meeting</t>
   </si>
+  <si>
+    <t>recheck location and dates in fall!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,16 +129,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -145,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -163,6 +164,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -224,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -259,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -436,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,18 +451,18 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="53.28515625" style="7" customWidth="1"/>
-    <col min="2" max="4" width="34.85546875" style="4" customWidth="1"/>
-    <col min="5" max="13" width="9.140625" style="4"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="53.33203125" style="7" customWidth="1"/>
+    <col min="2" max="4" width="34.83203125" style="4" customWidth="1"/>
+    <col min="5" max="13" width="8.83203125" style="4"/>
+    <col min="14" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -481,7 +485,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -495,7 +499,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -508,8 +512,11 @@
       <c r="D3" s="5">
         <v>43456</v>
       </c>
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -523,7 +530,7 @@
         <v>43532</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -531,6 +538,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added one item to prospective_conferences
</commit_message>
<xml_diff>
--- a/Prospective_Conferences_AY1819.xlsx
+++ b/Prospective_Conferences_AY1819.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Conference </t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>recheck location and dates in fall!</t>
+  </si>
+  <si>
+    <t>AEA / ASSA meetings</t>
+  </si>
+  <si>
+    <t>changes every year</t>
+  </si>
+  <si>
+    <t>January</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -167,6 +176,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -536,6 +548,20 @@
       </c>
       <c r="C5" s="5"/>
     </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9">
+        <v>43191</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
added new dates for Swiss conference
</commit_message>
<xml_diff>
--- a/Prospective_Conferences_AY1819.xlsx
+++ b/Prospective_Conferences_AY1819.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="26460" yWindow="700" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Conference </t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Modena, Italy</t>
-  </si>
-  <si>
-    <t>Lugano, Switzerland</t>
   </si>
   <si>
     <r>
@@ -68,9 +65,6 @@
     <t>Midwest macro Meeting</t>
   </si>
   <si>
-    <t>recheck location and dates in fall!</t>
-  </si>
-  <si>
     <t>AEA / ASSA meetings</t>
   </si>
   <si>
@@ -78,6 +72,9 @@
   </si>
   <si>
     <t>January</t>
+  </si>
+  <si>
+    <t>ETH Zürich, Switzerland</t>
   </si>
 </sst>
 </file>
@@ -452,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -463,7 +460,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -499,7 +496,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -513,24 +510,22 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5">
-        <v>43381</v>
+        <v>43380</v>
       </c>
       <c r="D3" s="5">
-        <v>43456</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>43455</v>
+      </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
@@ -544,22 +539,22 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9">
         <v>43191</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submitted to SEA (Swiss Economists Abroad) conference
</commit_message>
<xml_diff>
--- a/Prospective_Conferences_AY1819.xlsx
+++ b/Prospective_Conferences_AY1819.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26460" yWindow="700" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Conference </t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>ETH Zürich, Switzerland</t>
+  </si>
+  <si>
+    <t>Submitted on</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>See [SEA 2018] Submission ID 36.pdf</t>
   </si>
 </sst>
 </file>
@@ -171,11 +180,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,14 +469,16 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="53.33203125" style="7" customWidth="1"/>
     <col min="2" max="4" width="34.83203125" style="4" customWidth="1"/>
-    <col min="5" max="13" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="17.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="8.83203125" style="4"/>
     <col min="14" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -484,8 +495,12 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -521,7 +536,12 @@
       <c r="D3" s="5">
         <v>43455</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="9">
+        <v>43351</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="7" t="s">
@@ -550,7 +570,7 @@
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>43191</v>
       </c>
       <c r="D7" s="4" t="s">

</xml_diff>

<commit_message>
updated prospective conferences excel
included this MEA conference thingy
</commit_message>
<xml_diff>
--- a/Prospective_Conferences_AY1819.xlsx
+++ b/Prospective_Conferences_AY1819.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Conference </t>
   </si>
@@ -85,12 +85,24 @@
   <si>
     <t>See [SEA 2018] Submission ID 36.pdf</t>
   </si>
+  <si>
+    <t>MEA (Midwest Economic Association)</t>
+  </si>
+  <si>
+    <t>St Louis</t>
+  </si>
+  <si>
+    <t>Abstract submission for members only. Member fees: $20/year, abstract submission fee: $20, conference registration fee: $45, for non-members $135.</t>
+  </si>
+  <si>
+    <t>March 15-17, 2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +130,11 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Trebuchet MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -161,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -186,6 +203,7 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -577,6 +595,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>43381</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>